<commit_message>
New data structure and gen expression
</commit_message>
<xml_diff>
--- a/inst/app/data/data_set_list.xlsx
+++ b/inst/app/data/data_set_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
-  <si>
-    <t>Cerebral Organoids day 40</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>hPSC</t>
   </si>
@@ -30,21 +27,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>tables/CO day 40 vs hPSC.xlsx</t>
-  </si>
-  <si>
-    <t>Tendons</t>
-  </si>
-  <si>
-    <t>tendon</t>
-  </si>
-  <si>
-    <t>PSC</t>
-  </si>
-  <si>
-    <t>tables/tendon vs PSC.xlsx</t>
-  </si>
-  <si>
     <t>Dataset</t>
   </si>
   <si>
@@ -57,10 +39,103 @@
     <t>Condition2</t>
   </si>
   <si>
-    <t>This is a decription of the data set.</t>
-  </si>
-  <si>
-    <t>Cerebral Organoids day 40 compared to hPSC and this is a long wall of text. This shows that we can have a very verbose description of the data set amd it wil stil be displayed correctly in the app.  I write a few more words to make it even longer longer longer longer longer longer longer longer longer longer longer longer longer longer longer longer longer longer longer longer longer longer longer .</t>
+    <t>Cerebral Organoids day 40 compared to hPSC</t>
+  </si>
+  <si>
+    <t>NPC P1</t>
+  </si>
+  <si>
+    <t>NPC P3</t>
+  </si>
+  <si>
+    <t>NPC P5</t>
+  </si>
+  <si>
+    <t>Neural Crest d6</t>
+  </si>
+  <si>
+    <t>Sensory Neuron Diff d12</t>
+  </si>
+  <si>
+    <t>Sensory Neuron Maturation d18</t>
+  </si>
+  <si>
+    <t>Cerebral Organoids d40</t>
+  </si>
+  <si>
+    <t>Dorsal Forebrain d25</t>
+  </si>
+  <si>
+    <t>Dorsal Forebrain d50</t>
+  </si>
+  <si>
+    <t>Dorsal Forebrain d75</t>
+  </si>
+  <si>
+    <t>Ventral Forebrain d25</t>
+  </si>
+  <si>
+    <t>NPC at passage 1 in NPM</t>
+  </si>
+  <si>
+    <t>NPC at passage 3 in NPM</t>
+  </si>
+  <si>
+    <t>NPC at passage 5 in NPM</t>
+  </si>
+  <si>
+    <t>Neural Crest after day 6 differentiation</t>
+  </si>
+  <si>
+    <t>Sensory Neurons after 6 additional days of maturation</t>
+  </si>
+  <si>
+    <t>Sensory Neurons after 6 additional days of differentiation</t>
+  </si>
+  <si>
+    <t>Dorsal Forebrain Organoids at day 25</t>
+  </si>
+  <si>
+    <t>Dorsal Forebrain Organoids at day 75</t>
+  </si>
+  <si>
+    <t>Dorsal Forebrain Organoids at day 50</t>
+  </si>
+  <si>
+    <t>Ventral Forebrain Organoids at day 25</t>
+  </si>
+  <si>
+    <t>data/datasets/NPC_P1_vs_hPSC.Rds</t>
+  </si>
+  <si>
+    <t>data/datasets/NPC_P3_vs_hPSC.Rds</t>
+  </si>
+  <si>
+    <t>data/datasets/NPC_P5_vs_hPSC.Rds</t>
+  </si>
+  <si>
+    <t>data/datasets/Neural Crest_d6_vs_hPSC.Rds</t>
+  </si>
+  <si>
+    <t>data/datasets/Sensory Neuron Diff_d12_vs_hPSC.Rds</t>
+  </si>
+  <si>
+    <t>data/datasets/Sensory Neuron Maturation_d18_vs_hPSC.Rds</t>
+  </si>
+  <si>
+    <t>data/datasets/Cerebral Organoids_d40_vs_hPSC.Rds</t>
+  </si>
+  <si>
+    <t>data/datasets/Dorsal Forebrain_d25_vs_hPSC.Rds</t>
+  </si>
+  <si>
+    <t>data/datasets/Dorsal Forebrain_d50_vs_hPSC.Rds</t>
+  </si>
+  <si>
+    <t>data/datasets/Dorsal Forebrain_d75_vs_hPSC.Rds</t>
+  </si>
+  <si>
+    <t>data/datasets/Ventral Forebrain_d25_vs_hPSC.Rds</t>
   </si>
 </sst>
 </file>
@@ -394,15 +469,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
@@ -411,55 +486,208 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename columns and split dataset input
</commit_message>
<xml_diff>
--- a/inst/app/data/data_set_list.xlsx
+++ b/inst/app/data/data_set_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="7440" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>hPSC</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>Ventral Forebrain Organoids at day 25  compared to hPSC</t>
+  </si>
+  <si>
+    <t>Input_group</t>
+  </si>
+  <si>
+    <t>2D Media</t>
+  </si>
+  <si>
+    <t>Organoid Media</t>
   </si>
 </sst>
 </file>
@@ -453,13 +462,13 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="49.140625" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
@@ -479,9 +488,11 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -498,6 +509,9 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -515,6 +529,9 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -532,6 +549,9 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -549,6 +569,9 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -566,6 +589,9 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -583,6 +609,9 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>